<commit_message>
[MS-OXORULE]: Update RS blocked by TDI.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXORULE/MS-OXORULE_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXORULE/MS-OXORULE_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5860" uniqueCount="1885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5857" uniqueCount="1885">
   <si>
     <t>Req ID</t>
   </si>
@@ -5947,7 +5947,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -7179,7 +7179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7212,9 +7212,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7247,6 +7264,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7426,9 +7460,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L821"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A738" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A743" sqref="A743:XFD743"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -15491,7 +15523,7 @@
         <v>15</v>
       </c>
       <c r="H324" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I324" s="31"/>
     </row>
@@ -15516,7 +15548,7 @@
         <v>15</v>
       </c>
       <c r="H325" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I325" s="31"/>
     </row>
@@ -15595,7 +15627,7 @@
         <v>15</v>
       </c>
       <c r="H328" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I328" s="31"/>
     </row>
@@ -15699,7 +15731,7 @@
         <v>15</v>
       </c>
       <c r="H332" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I332" s="31"/>
     </row>
@@ -15749,7 +15781,7 @@
         <v>15</v>
       </c>
       <c r="H334" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I334" s="31"/>
     </row>
@@ -15899,7 +15931,7 @@
         <v>15</v>
       </c>
       <c r="H340" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I340" s="31"/>
     </row>
@@ -18479,7 +18511,7 @@
         <v>15</v>
       </c>
       <c r="H442" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I442" s="31"/>
     </row>
@@ -18504,7 +18536,7 @@
         <v>15</v>
       </c>
       <c r="H443" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I443" s="31"/>
     </row>
@@ -18529,7 +18561,7 @@
         <v>15</v>
       </c>
       <c r="H444" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I444" s="31"/>
     </row>
@@ -18554,7 +18586,7 @@
         <v>15</v>
       </c>
       <c r="H445" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I445" s="31"/>
     </row>
@@ -18579,7 +18611,7 @@
         <v>15</v>
       </c>
       <c r="H446" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I446" s="31"/>
     </row>
@@ -18629,7 +18661,7 @@
         <v>15</v>
       </c>
       <c r="H448" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I448" s="31"/>
     </row>
@@ -18654,7 +18686,7 @@
         <v>15</v>
       </c>
       <c r="H449" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I449" s="31"/>
     </row>
@@ -18679,7 +18711,7 @@
         <v>15</v>
       </c>
       <c r="H450" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I450" s="31"/>
     </row>
@@ -18704,7 +18736,7 @@
         <v>15</v>
       </c>
       <c r="H451" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I451" s="31"/>
     </row>
@@ -18729,7 +18761,7 @@
         <v>15</v>
       </c>
       <c r="H452" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I452" s="31"/>
     </row>
@@ -18754,7 +18786,7 @@
         <v>15</v>
       </c>
       <c r="H453" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I453" s="31"/>
     </row>
@@ -18779,7 +18811,7 @@
         <v>15</v>
       </c>
       <c r="H454" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I454" s="31"/>
     </row>
@@ -18804,7 +18836,7 @@
         <v>15</v>
       </c>
       <c r="H455" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I455" s="31"/>
     </row>
@@ -18904,7 +18936,7 @@
         <v>15</v>
       </c>
       <c r="H459" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I459" s="31"/>
     </row>
@@ -19004,7 +19036,7 @@
         <v>15</v>
       </c>
       <c r="H463" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I463" s="31"/>
     </row>
@@ -25474,11 +25506,9 @@
         <v>15</v>
       </c>
       <c r="H717" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I717" s="20" t="s">
-        <v>1511</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I717" s="20"/>
     </row>
     <row r="718" spans="1:9" ht="30">
       <c r="A718" s="29" t="s">
@@ -26061,11 +26091,9 @@
         <v>15</v>
       </c>
       <c r="H738" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="I738" s="31" t="s">
-        <v>1511</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I738" s="31"/>
     </row>
     <row r="739" spans="1:9" ht="45">
       <c r="A739" s="22" t="s">
@@ -26090,11 +26118,9 @@
         <v>15</v>
       </c>
       <c r="H739" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="I739" s="31" t="s">
-        <v>1511</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I739" s="31"/>
     </row>
     <row r="740" spans="1:9" ht="45">
       <c r="A740" s="29" t="s">

</xml_diff>

<commit_message>
Update rs528 to non-testable
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXORULE/MS-OXORULE_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXORULE/MS-OXORULE_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5857" uniqueCount="1885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5858" uniqueCount="1886">
   <si>
     <t>Req ID</t>
   </si>
@@ -5943,11 +5943,14 @@
   <si>
     <t>[[In Appendix A: Product Behavior] Implementation does set this value [Reserved (1 byte)] to 0x00. [&lt;9&gt; Section 2.2.5.1.2.4.1: Exchange 2010, Exchange 2013, and Exchange 2016 set this value to 0x00.]</t>
   </si>
+  <si>
+    <t>Verified by requirement: MS-OXORULE_R5281.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -6268,6 +6271,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6292,26 +6310,41 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="83">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -7089,34 +7122,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I818" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I818" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
   <autoFilter ref="A19:I818"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="21">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="20">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="19">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="18">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="17">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -7125,12 +7158,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Scope" dataDxfId="8"/>
+    <tableColumn id="2" name="Test" dataDxfId="7"/>
+    <tableColumn id="3" name="Description" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7179,7 +7212,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7212,26 +7245,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7264,23 +7280,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7460,7 +7459,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L821"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A617" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A621" sqref="A621"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -7514,127 +7515,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -7647,12 +7648,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -7665,12 +7666,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -7683,12 +7684,12 @@
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -7701,60 +7702,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -22941,7 +22942,7 @@
       <c r="H618" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I618" s="31" t="s">
+      <c r="I618" s="20" t="s">
         <v>1495</v>
       </c>
     </row>
@@ -23016,9 +23017,11 @@
         <v>15</v>
       </c>
       <c r="H621" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I621" s="31"/>
+        <v>17</v>
+      </c>
+      <c r="I621" s="20" t="s">
+        <v>1885</v>
+      </c>
     </row>
     <row r="622" spans="1:9" ht="45">
       <c r="A622" s="29" t="s">
@@ -28218,11 +28221,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -28230,221 +28228,226 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A235:I238 E34:I233 A20:H233 A819:I819 I771:I819 A240:I817">
-    <cfRule type="expression" dxfId="76" priority="1099">
+    <cfRule type="expression" dxfId="82" priority="1099">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="1100">
+    <cfRule type="expression" dxfId="81" priority="1100">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="1107">
+    <cfRule type="expression" dxfId="80" priority="1107">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A235:I238 E34:I233 A20:H233 A819:I819 I771:I819 A240:I817">
-    <cfRule type="expression" dxfId="73" priority="1053">
+    <cfRule type="expression" dxfId="79" priority="1053">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="1054">
+    <cfRule type="expression" dxfId="78" priority="1054">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="1055">
+    <cfRule type="expression" dxfId="77" priority="1055">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F233 F235:F238 F819 F240:F817">
-    <cfRule type="expression" dxfId="70" priority="1059">
+    <cfRule type="expression" dxfId="76" priority="1059">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="1060">
+    <cfRule type="expression" dxfId="75" priority="1060">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I233 I235:I238">
-    <cfRule type="expression" dxfId="68" priority="1050">
+    <cfRule type="expression" dxfId="74" priority="1050">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="1051">
+    <cfRule type="expression" dxfId="73" priority="1051">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="1052">
+    <cfRule type="expression" dxfId="72" priority="1052">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I233 I235:I238">
-    <cfRule type="expression" dxfId="65" priority="1047">
+    <cfRule type="expression" dxfId="71" priority="1047">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="1048">
+    <cfRule type="expression" dxfId="70" priority="1048">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="1049">
+    <cfRule type="expression" dxfId="69" priority="1049">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A234:J234">
-    <cfRule type="expression" dxfId="62" priority="1044">
+    <cfRule type="expression" dxfId="68" priority="1044">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="1045">
+    <cfRule type="expression" dxfId="67" priority="1045">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="1046">
+    <cfRule type="expression" dxfId="66" priority="1046">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A234:J234">
-    <cfRule type="expression" dxfId="59" priority="1039">
+    <cfRule type="expression" dxfId="65" priority="1039">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="1040">
+    <cfRule type="expression" dxfId="64" priority="1040">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="1041">
+    <cfRule type="expression" dxfId="63" priority="1041">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F234">
-    <cfRule type="expression" dxfId="56" priority="1042">
+    <cfRule type="expression" dxfId="62" priority="1042">
       <formula>NOT(VLOOKUP(F234,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="1043">
+    <cfRule type="expression" dxfId="61" priority="1043">
       <formula>(VLOOKUP(F234,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A239:J239">
-    <cfRule type="expression" dxfId="54" priority="1036">
+    <cfRule type="expression" dxfId="60" priority="1036">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="1037">
+    <cfRule type="expression" dxfId="59" priority="1037">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="1038">
+    <cfRule type="expression" dxfId="58" priority="1038">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A239:J239">
-    <cfRule type="expression" dxfId="51" priority="1031">
+    <cfRule type="expression" dxfId="57" priority="1031">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="1032">
+    <cfRule type="expression" dxfId="56" priority="1032">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="1033">
+    <cfRule type="expression" dxfId="55" priority="1033">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F239">
-    <cfRule type="expression" dxfId="48" priority="1034">
+    <cfRule type="expression" dxfId="54" priority="1034">
       <formula>NOT(VLOOKUP(F239,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="1035">
+    <cfRule type="expression" dxfId="53" priority="1035">
       <formula>(VLOOKUP(F239,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B818:H818">
-    <cfRule type="expression" dxfId="46" priority="1028">
+    <cfRule type="expression" dxfId="52" priority="1028">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="1029">
+    <cfRule type="expression" dxfId="51" priority="1029">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="1030">
+    <cfRule type="expression" dxfId="50" priority="1030">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B818:H818">
-    <cfRule type="expression" dxfId="43" priority="1023">
+    <cfRule type="expression" dxfId="49" priority="1023">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="1024">
+    <cfRule type="expression" dxfId="48" priority="1024">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="1025">
+    <cfRule type="expression" dxfId="47" priority="1025">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F818">
-    <cfRule type="expression" dxfId="40" priority="1026">
+    <cfRule type="expression" dxfId="46" priority="1026">
       <formula>NOT(VLOOKUP(F818,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="1027">
+    <cfRule type="expression" dxfId="45" priority="1027">
       <formula>(VLOOKUP(F818,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F818">
-    <cfRule type="expression" dxfId="38" priority="1021">
+    <cfRule type="expression" dxfId="44" priority="1021">
       <formula>NOT(VLOOKUP(F818,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="1022">
+    <cfRule type="expression" dxfId="43" priority="1022">
       <formula>(VLOOKUP(F818,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B818">
-    <cfRule type="expression" dxfId="36" priority="1018">
+    <cfRule type="expression" dxfId="42" priority="1018">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="1019">
+    <cfRule type="expression" dxfId="41" priority="1019">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="1020">
+    <cfRule type="expression" dxfId="40" priority="1020">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B818">
-    <cfRule type="expression" dxfId="33" priority="1015">
+    <cfRule type="expression" dxfId="39" priority="1015">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="1016">
+    <cfRule type="expression" dxfId="38" priority="1016">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="1017">
+    <cfRule type="expression" dxfId="37" priority="1017">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C818">
-    <cfRule type="expression" dxfId="30" priority="1012">
+    <cfRule type="expression" dxfId="36" priority="1012">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="1013">
+    <cfRule type="expression" dxfId="35" priority="1013">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="1014">
+    <cfRule type="expression" dxfId="34" priority="1014">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C818">
-    <cfRule type="expression" dxfId="27" priority="1009">
+    <cfRule type="expression" dxfId="33" priority="1009">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="1010">
+    <cfRule type="expression" dxfId="32" priority="1010">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="1011">
+    <cfRule type="expression" dxfId="31" priority="1011">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A818">
-    <cfRule type="expression" dxfId="24" priority="1006">
+    <cfRule type="expression" dxfId="30" priority="1006">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="1007">
+    <cfRule type="expression" dxfId="29" priority="1007">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="1008">
+    <cfRule type="expression" dxfId="28" priority="1008">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A818">
-    <cfRule type="expression" dxfId="21" priority="1003">
+    <cfRule type="expression" dxfId="27" priority="1003">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="1004">
+    <cfRule type="expression" dxfId="26" priority="1004">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="1005">
+    <cfRule type="expression" dxfId="25" priority="1005">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update r7131 to unverified
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXORULE/MS-OXORULE_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXORULE/MS-OXORULE_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5858" uniqueCount="1886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5857" uniqueCount="1886">
   <si>
     <t>Req ID</t>
   </si>
@@ -6271,21 +6271,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6310,41 +6295,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="83">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="77">
     <dxf>
       <font>
         <b val="0"/>
@@ -7122,34 +7092,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I818" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I818" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I818"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="22">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="21">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="20">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="19">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="18">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="17">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="16">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="15">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="14">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -7158,12 +7128,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="8"/>
-    <tableColumn id="2" name="Test" dataDxfId="7"/>
-    <tableColumn id="3" name="Description" dataDxfId="6"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7459,13 +7429,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L821"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A617" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A621" sqref="A621"/>
+    <sheetView tabSelected="1" topLeftCell="A744" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C748" sqref="C748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
@@ -7515,127 +7485,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -7648,12 +7618,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -7666,12 +7636,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -7684,12 +7654,12 @@
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -7702,60 +7672,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -26320,11 +26290,9 @@
         <v>15</v>
       </c>
       <c r="H746" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="I746" s="31" t="s">
-        <v>1511</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I746" s="31"/>
     </row>
     <row r="747" spans="1:9" ht="60">
       <c r="A747" s="22" t="s">
@@ -28221,6 +28189,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -28228,226 +28201,221 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A235:I238 E34:I233 A20:H233 A819:I819 I771:I819 A240:I817">
-    <cfRule type="expression" dxfId="82" priority="1099">
+    <cfRule type="expression" dxfId="76" priority="1099">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="1100">
+    <cfRule type="expression" dxfId="75" priority="1100">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="1107">
+    <cfRule type="expression" dxfId="74" priority="1107">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A235:I238 E34:I233 A20:H233 A819:I819 I771:I819 A240:I817">
-    <cfRule type="expression" dxfId="79" priority="1053">
+    <cfRule type="expression" dxfId="73" priority="1053">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="1054">
+    <cfRule type="expression" dxfId="72" priority="1054">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="1055">
+    <cfRule type="expression" dxfId="71" priority="1055">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F233 F235:F238 F819 F240:F817">
-    <cfRule type="expression" dxfId="76" priority="1059">
+    <cfRule type="expression" dxfId="70" priority="1059">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="1060">
+    <cfRule type="expression" dxfId="69" priority="1060">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I233 I235:I238">
-    <cfRule type="expression" dxfId="74" priority="1050">
+    <cfRule type="expression" dxfId="68" priority="1050">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="1051">
+    <cfRule type="expression" dxfId="67" priority="1051">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="1052">
+    <cfRule type="expression" dxfId="66" priority="1052">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I233 I235:I238">
-    <cfRule type="expression" dxfId="71" priority="1047">
+    <cfRule type="expression" dxfId="65" priority="1047">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="1048">
+    <cfRule type="expression" dxfId="64" priority="1048">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="1049">
+    <cfRule type="expression" dxfId="63" priority="1049">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A234:J234">
-    <cfRule type="expression" dxfId="68" priority="1044">
+    <cfRule type="expression" dxfId="62" priority="1044">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="1045">
+    <cfRule type="expression" dxfId="61" priority="1045">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="1046">
+    <cfRule type="expression" dxfId="60" priority="1046">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A234:J234">
-    <cfRule type="expression" dxfId="65" priority="1039">
+    <cfRule type="expression" dxfId="59" priority="1039">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="1040">
+    <cfRule type="expression" dxfId="58" priority="1040">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="1041">
+    <cfRule type="expression" dxfId="57" priority="1041">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F234">
-    <cfRule type="expression" dxfId="62" priority="1042">
+    <cfRule type="expression" dxfId="56" priority="1042">
       <formula>NOT(VLOOKUP(F234,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="1043">
+    <cfRule type="expression" dxfId="55" priority="1043">
       <formula>(VLOOKUP(F234,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A239:J239">
-    <cfRule type="expression" dxfId="60" priority="1036">
+    <cfRule type="expression" dxfId="54" priority="1036">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="1037">
+    <cfRule type="expression" dxfId="53" priority="1037">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="1038">
+    <cfRule type="expression" dxfId="52" priority="1038">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A239:J239">
-    <cfRule type="expression" dxfId="57" priority="1031">
+    <cfRule type="expression" dxfId="51" priority="1031">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="1032">
+    <cfRule type="expression" dxfId="50" priority="1032">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="1033">
+    <cfRule type="expression" dxfId="49" priority="1033">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F239">
-    <cfRule type="expression" dxfId="54" priority="1034">
+    <cfRule type="expression" dxfId="48" priority="1034">
       <formula>NOT(VLOOKUP(F239,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="1035">
+    <cfRule type="expression" dxfId="47" priority="1035">
       <formula>(VLOOKUP(F239,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B818:H818">
-    <cfRule type="expression" dxfId="52" priority="1028">
+    <cfRule type="expression" dxfId="46" priority="1028">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="1029">
+    <cfRule type="expression" dxfId="45" priority="1029">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="1030">
+    <cfRule type="expression" dxfId="44" priority="1030">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B818:H818">
-    <cfRule type="expression" dxfId="49" priority="1023">
+    <cfRule type="expression" dxfId="43" priority="1023">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="1024">
+    <cfRule type="expression" dxfId="42" priority="1024">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="1025">
+    <cfRule type="expression" dxfId="41" priority="1025">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F818">
-    <cfRule type="expression" dxfId="46" priority="1026">
+    <cfRule type="expression" dxfId="40" priority="1026">
       <formula>NOT(VLOOKUP(F818,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="1027">
+    <cfRule type="expression" dxfId="39" priority="1027">
       <formula>(VLOOKUP(F818,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F818">
-    <cfRule type="expression" dxfId="44" priority="1021">
+    <cfRule type="expression" dxfId="38" priority="1021">
       <formula>NOT(VLOOKUP(F818,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="1022">
+    <cfRule type="expression" dxfId="37" priority="1022">
       <formula>(VLOOKUP(F818,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B818">
-    <cfRule type="expression" dxfId="42" priority="1018">
+    <cfRule type="expression" dxfId="36" priority="1018">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="1019">
+    <cfRule type="expression" dxfId="35" priority="1019">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="1020">
+    <cfRule type="expression" dxfId="34" priority="1020">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B818">
-    <cfRule type="expression" dxfId="39" priority="1015">
+    <cfRule type="expression" dxfId="33" priority="1015">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="1016">
+    <cfRule type="expression" dxfId="32" priority="1016">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="1017">
+    <cfRule type="expression" dxfId="31" priority="1017">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C818">
-    <cfRule type="expression" dxfId="36" priority="1012">
+    <cfRule type="expression" dxfId="30" priority="1012">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="1013">
+    <cfRule type="expression" dxfId="29" priority="1013">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="1014">
+    <cfRule type="expression" dxfId="28" priority="1014">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C818">
-    <cfRule type="expression" dxfId="33" priority="1009">
+    <cfRule type="expression" dxfId="27" priority="1009">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="1010">
+    <cfRule type="expression" dxfId="26" priority="1010">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="1011">
+    <cfRule type="expression" dxfId="25" priority="1011">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A818">
-    <cfRule type="expression" dxfId="30" priority="1006">
+    <cfRule type="expression" dxfId="24" priority="1006">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="1007">
+    <cfRule type="expression" dxfId="23" priority="1007">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="1008">
+    <cfRule type="expression" dxfId="22" priority="1008">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A818">
-    <cfRule type="expression" dxfId="27" priority="1003">
+    <cfRule type="expression" dxfId="21" priority="1003">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="1004">
+    <cfRule type="expression" dxfId="20" priority="1004">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="1005">
+    <cfRule type="expression" dxfId="19" priority="1005">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>